<commit_message>
Made Image transparent and added Image-Loader
</commit_message>
<xml_diff>
--- a/Checkers.xlsx
+++ b/Checkers.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6F2DDF-A351-4395-88A6-7D4FEC6E63AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GUI" sheetId="1" r:id="rId1"/>
-    <sheet name="Game" sheetId="2" r:id="rId2"/>
-    <sheet name="Player" sheetId="3" r:id="rId3"/>
-    <sheet name="Checker" sheetId="4" r:id="rId4"/>
-    <sheet name="King" sheetId="5" r:id="rId5"/>
+    <sheet name="Diagramm" sheetId="7" r:id="rId1"/>
+    <sheet name="GUI" sheetId="6" r:id="rId2"/>
+    <sheet name="Game" sheetId="2" r:id="rId3"/>
+    <sheet name="Player" sheetId="3" r:id="rId4"/>
+    <sheet name="Checker" sheetId="4" r:id="rId5"/>
+    <sheet name="King extends Checker" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Methode</t>
   </si>
@@ -39,11 +41,29 @@
   <si>
     <t>public static void main</t>
   </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>Erzeugt zwei Instanzen der Klasse Player</t>
+  </si>
+  <si>
+    <t>GUI mit Eingabemaske</t>
+  </si>
+  <si>
+    <t>newGame()</t>
+  </si>
+  <si>
+    <t>Erzeugt neue Instanz der Klasse Game und übergibt Start Parameter</t>
+  </si>
+  <si>
+    <t>Erzeugt 10 Instanzen der Klasse Checker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,12 +81,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -99,6 +126,926 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Ellipse 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC73035-69A7-4521-801A-274970953DCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="295275"/>
+          <a:ext cx="2638425" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="2000"/>
+            <a:t>GUI</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Ellipse 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C75B6B1-0E5C-484F-B9DF-9F9350BDFAB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4133850" y="876300"/>
+          <a:ext cx="2638425" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="2000"/>
+            <a:t>Game</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Ellipse 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{606DC0BC-199F-453C-8D65-3F92618742CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="2524125"/>
+          <a:ext cx="2638425" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="2000"/>
+            <a:t>Player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Ellipse 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3620C74B-52A4-4AAB-AFBE-F565DD77F0F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953250" y="2524125"/>
+          <a:ext cx="2638425" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="2000"/>
+            <a:t>Player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Ellipse 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F19B89E-D04A-4C0C-86A4-C8113F6F1A7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="457201" y="4600575"/>
+          <a:ext cx="2162174" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600"/>
+            <a:t>Checker =&gt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600" baseline="0"/>
+            <a:t> 10x</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-CH" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Ellipse 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F2BCCEC-72CC-4FEA-A51E-1BD9CA3561A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867401" y="4524375"/>
+          <a:ext cx="2162174" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600"/>
+            <a:t>Checker =&gt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600" baseline="0"/>
+            <a:t> 10x</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-CH" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Ellipse 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81FCBA2F-58F4-4FAF-BEF0-D46BA930A425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8915401" y="4524375"/>
+          <a:ext cx="2162174" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600"/>
+            <a:t>King</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Ellipse 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B72A52B2-2834-4B4E-BC26-F384114D098C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3371851" y="4591050"/>
+          <a:ext cx="2162174" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1600"/>
+            <a:t>King</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Gerade Verbindung mit Pfeil 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92470972-6829-4C63-A87C-207E11EC4AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2981325" y="1004888"/>
+          <a:ext cx="1152525" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>80337</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>710238</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Gerade Verbindung mit Pfeil 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B18DF22-B605-4476-B100-811F72868103}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="4" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3890337" y="2087684"/>
+          <a:ext cx="629901" cy="644282"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>289887</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>481638</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Gerade Verbindung mit Pfeil 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5A85D1-61F1-4E8A-9243-140DD129929D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="5"/>
+          <a:endCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6385887" y="2087684"/>
+          <a:ext cx="953751" cy="644282"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>500688</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Gerade Verbindung mit Pfeil 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7694CF7-6B26-469F-87C9-08CA7ABC7C93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1538288" y="3735509"/>
+          <a:ext cx="486400" cy="865066"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Gerade Verbindung mit Pfeil 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D59A5F-9BEB-4EFA-BF9F-7B5A28930139}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="6"/>
+          <a:endCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2619375" y="5224463"/>
+          <a:ext cx="752476" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>90488</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>481638</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Gerade Verbindung mit Pfeil 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA33DC1-8E98-4099-A844-B2611EA02592}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6948488" y="3735509"/>
+          <a:ext cx="391150" cy="788866"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Gerade Verbindung mit Pfeil 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26F1C36-C0EB-4B8F-B0F7-E98E62F84700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8029575" y="5157788"/>
+          <a:ext cx="885826" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,12 +1310,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C502A4-7924-475F-B728-0F0619BE68B1}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F830EF7-043E-4D31-944A-A3BA8DE9EC88}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="107.140625" customWidth="1"/>
@@ -394,57 +1357,135 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="107.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="107.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="107.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="107.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>